<commit_message>
updated signals with the same name (ie. gnd)
</commit_message>
<xml_diff>
--- a/Excel Sheet/Clock Chip.xlsx
+++ b/Excel Sheet/Clock Chip.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="135" windowWidth="23955" windowHeight="9780" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="135" windowWidth="21720" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Signals" sheetId="1" r:id="rId1"/>
@@ -12,14 +12,15 @@
     <sheet name="Capture Sorted" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Capture Sorted'!$K$3:$O$22</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Signals!$B$3:$E$59</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="111">
   <si>
     <t>Pin #</t>
   </si>
@@ -337,6 +338,21 @@
   </si>
   <si>
     <t>Line</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VDD_SRC_I/O_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VDD_SRC_I/O_2</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VSS_SRC_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> VSS_SRC_2</t>
+  </si>
+  <si>
+    <t>z</t>
   </si>
 </sst>
 </file>
@@ -1941,11 +1957,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:AA22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="T4" sqref="T4:X21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="18.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:27" ht="18.75">
       <c r="B2" s="4" t="s">
@@ -2034,31 +2055,31 @@
     </row>
     <row r="4" spans="2:27">
       <c r="B4">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D4" t="s">
         <v>104</v>
       </c>
       <c r="E4">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
         <v>105</v>
       </c>
-      <c r="K4">
-        <v>10</v>
+      <c r="K4" t="s">
+        <v>110</v>
       </c>
       <c r="L4" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
       <c r="M4" t="s">
         <v>104</v>
       </c>
       <c r="N4">
-        <v>1</v>
+        <v>16</v>
       </c>
       <c r="O4" t="s">
         <v>105</v>
@@ -2081,31 +2102,31 @@
     </row>
     <row r="5" spans="2:27">
       <c r="B5">
-        <v>8</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+      <c r="E5">
         <v>18</v>
       </c>
-      <c r="D5" t="s">
-        <v>104</v>
-      </c>
-      <c r="E5">
-        <v>2</v>
-      </c>
       <c r="F5" t="s">
         <v>105</v>
       </c>
       <c r="K5">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="L5" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="M5" t="s">
         <v>104</v>
       </c>
       <c r="N5">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="O5" t="s">
         <v>105</v>
@@ -2128,31 +2149,31 @@
     </row>
     <row r="6" spans="2:27">
       <c r="B6">
-        <v>11</v>
+        <v>41</v>
       </c>
       <c r="C6" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
         <v>104</v>
       </c>
       <c r="E6">
-        <v>3</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
         <v>105</v>
       </c>
       <c r="K6">
-        <v>1</v>
+        <v>49</v>
       </c>
       <c r="L6" t="s">
-        <v>4</v>
+        <v>77</v>
       </c>
       <c r="M6" t="s">
         <v>104</v>
       </c>
       <c r="N6">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="O6" t="s">
         <v>105</v>
@@ -2175,31 +2196,31 @@
     </row>
     <row r="7" spans="2:27">
       <c r="B7">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>36</v>
+        <v>26</v>
       </c>
       <c r="D7" t="s">
         <v>104</v>
       </c>
       <c r="E7">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
         <v>105</v>
       </c>
       <c r="K7">
-        <v>3</v>
+        <v>40</v>
       </c>
       <c r="L7" t="s">
-        <v>10</v>
+        <v>65</v>
       </c>
       <c r="M7" t="s">
         <v>104</v>
       </c>
       <c r="N7">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="O7" t="s">
         <v>105</v>
@@ -2222,31 +2243,31 @@
     </row>
     <row r="8" spans="2:27">
       <c r="B8">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="D8" t="s">
         <v>104</v>
       </c>
       <c r="E8">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="F8" t="s">
         <v>105</v>
       </c>
       <c r="K8">
+        <v>1</v>
+      </c>
+      <c r="L8" t="s">
         <v>4</v>
       </c>
-      <c r="L8" t="s">
-        <v>11</v>
-      </c>
       <c r="M8" t="s">
         <v>104</v>
       </c>
       <c r="N8">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O8" t="s">
         <v>105</v>
@@ -2269,31 +2290,31 @@
     </row>
     <row r="9" spans="2:27">
       <c r="B9">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D9" t="s">
         <v>104</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="F9" t="s">
         <v>105</v>
       </c>
       <c r="K9">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="L9" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="M9" t="s">
         <v>104</v>
       </c>
       <c r="N9">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="O9" t="s">
         <v>105</v>
@@ -2316,31 +2337,31 @@
     </row>
     <row r="10" spans="2:27">
       <c r="B10">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>37</v>
       </c>
       <c r="D10" t="s">
         <v>104</v>
       </c>
       <c r="E10">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
         <v>105</v>
       </c>
       <c r="K10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="L10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M10" t="s">
         <v>104</v>
       </c>
       <c r="N10">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="O10" t="s">
         <v>105</v>
@@ -2363,31 +2384,31 @@
     </row>
     <row r="11" spans="2:27">
       <c r="B11">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C11" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
         <v>104</v>
       </c>
       <c r="E11">
-        <v>8</v>
+        <v>19</v>
       </c>
       <c r="F11" t="s">
         <v>105</v>
       </c>
       <c r="K11">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="L11" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="M11" t="s">
         <v>104</v>
       </c>
       <c r="N11">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="O11" t="s">
         <v>105</v>
@@ -2410,31 +2431,31 @@
     </row>
     <row r="12" spans="2:27">
       <c r="B12">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" t="s">
+        <v>104</v>
+      </c>
+      <c r="E12">
         <v>12</v>
       </c>
-      <c r="C12" t="s">
-        <v>26</v>
-      </c>
-      <c r="D12" t="s">
-        <v>104</v>
-      </c>
-      <c r="E12">
-        <v>9</v>
-      </c>
       <c r="F12" t="s">
         <v>105</v>
       </c>
       <c r="K12">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="L12" t="s">
-        <v>44</v>
+        <v>17</v>
       </c>
       <c r="M12" t="s">
         <v>104</v>
       </c>
       <c r="N12">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="O12" t="s">
         <v>105</v>
@@ -2457,31 +2478,31 @@
     </row>
     <row r="13" spans="2:27">
       <c r="B13">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>106</v>
       </c>
       <c r="D13" t="s">
         <v>104</v>
       </c>
       <c r="E13">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
         <v>105</v>
       </c>
       <c r="K13">
-        <v>29</v>
+        <v>54</v>
       </c>
       <c r="L13" t="s">
-        <v>49</v>
+        <v>84</v>
       </c>
       <c r="M13" t="s">
         <v>104</v>
       </c>
       <c r="N13">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="O13" t="s">
         <v>105</v>
@@ -2504,31 +2525,31 @@
     </row>
     <row r="14" spans="2:27">
       <c r="B14">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
         <v>104</v>
       </c>
       <c r="E14">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F14" t="s">
         <v>105</v>
       </c>
       <c r="K14">
-        <v>30</v>
+        <v>56</v>
       </c>
       <c r="L14" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="M14" t="s">
         <v>104</v>
       </c>
       <c r="N14">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="O14" t="s">
         <v>105</v>
@@ -2551,31 +2572,31 @@
     </row>
     <row r="15" spans="2:27">
       <c r="B15">
-        <v>31</v>
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>56</v>
+        <v>25</v>
       </c>
       <c r="D15" t="s">
         <v>104</v>
       </c>
       <c r="E15">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="F15" t="s">
         <v>105</v>
       </c>
       <c r="K15">
-        <v>35</v>
+        <v>55</v>
       </c>
       <c r="L15" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="M15" t="s">
         <v>104</v>
       </c>
       <c r="N15">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O15" t="s">
         <v>105</v>
@@ -2598,31 +2619,31 @@
     </row>
     <row r="16" spans="2:27">
       <c r="B16">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>45</v>
+        <v>71</v>
       </c>
       <c r="D16" t="s">
         <v>104</v>
       </c>
       <c r="E16">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="F16" t="s">
         <v>105</v>
       </c>
       <c r="K16">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="L16" t="s">
-        <v>61</v>
+        <v>44</v>
       </c>
       <c r="M16" t="s">
         <v>104</v>
       </c>
       <c r="N16">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="O16" t="s">
         <v>105</v>
@@ -2645,31 +2666,31 @@
     </row>
     <row r="17" spans="2:24">
       <c r="B17">
-        <v>41</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="D17" t="s">
         <v>104</v>
       </c>
       <c r="E17">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
         <v>105</v>
       </c>
       <c r="K17">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="L17" t="s">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="M17" t="s">
         <v>104</v>
       </c>
       <c r="N17">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="O17" t="s">
         <v>105</v>
@@ -2692,31 +2713,31 @@
     </row>
     <row r="18" spans="2:24">
       <c r="B18">
+        <v>8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" t="s">
+        <v>104</v>
+      </c>
+      <c r="E18">
         <v>2</v>
       </c>
-      <c r="C18" t="s">
-        <v>7</v>
-      </c>
-      <c r="D18" t="s">
-        <v>104</v>
-      </c>
-      <c r="E18">
-        <v>15</v>
-      </c>
       <c r="F18" t="s">
         <v>105</v>
       </c>
       <c r="K18">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="L18" t="s">
-        <v>86</v>
+        <v>60</v>
       </c>
       <c r="M18" t="s">
         <v>104</v>
       </c>
       <c r="N18">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O18" t="s">
         <v>105</v>
@@ -2739,31 +2760,31 @@
     </row>
     <row r="19" spans="2:24">
       <c r="B19">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="C19" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="D19" t="s">
         <v>104</v>
       </c>
       <c r="E19">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="F19" t="s">
         <v>105</v>
       </c>
       <c r="K19">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="L19" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="M19" t="s">
         <v>104</v>
       </c>
       <c r="N19">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="O19" t="s">
         <v>105</v>
@@ -2786,31 +2807,31 @@
     </row>
     <row r="20" spans="2:24">
       <c r="B20">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="D20" t="s">
         <v>104</v>
       </c>
       <c r="E20">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F20" t="s">
         <v>105</v>
       </c>
       <c r="K20">
-        <v>49</v>
+        <v>4</v>
       </c>
       <c r="L20" t="s">
-        <v>77</v>
+        <v>11</v>
       </c>
       <c r="M20" t="s">
         <v>104</v>
       </c>
       <c r="N20">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="O20" t="s">
         <v>105</v>
@@ -2833,31 +2854,31 @@
     </row>
     <row r="21" spans="2:24">
       <c r="B21">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="D21" t="s">
         <v>104</v>
       </c>
       <c r="E21">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="F21" t="s">
         <v>105</v>
       </c>
       <c r="K21">
-        <v>52</v>
+        <v>10</v>
       </c>
       <c r="L21" t="s">
-        <v>82</v>
+        <v>22</v>
       </c>
       <c r="M21" t="s">
         <v>104</v>
       </c>
       <c r="N21">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="O21" t="s">
         <v>105</v>
@@ -2880,37 +2901,42 @@
     </row>
     <row r="22" spans="2:24">
       <c r="B22">
-        <v>53</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="D22" t="s">
         <v>104</v>
       </c>
       <c r="E22">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="F22" t="s">
         <v>105</v>
       </c>
       <c r="K22">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="L22" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="M22" t="s">
         <v>104</v>
       </c>
       <c r="N22">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="O22" t="s">
         <v>105</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="K3:O22">
+    <sortState ref="K4:O22">
+      <sortCondition ref="L3:L22"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>